<commit_message>
MCD et dictionnaire finis
</commit_message>
<xml_diff>
--- a/Livrable-2/Dictionnaire de données.xlsx
+++ b/Livrable-2/Dictionnaire de données.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schne\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://viacesifr-my.sharepoint.com/personal/anthony_schnepp_viacesi_fr/Documents/Bureau/Études One Drive/A2/Projets/Programmation orientée objet/Livrable 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580B3F30-1DBD-4438-AD19-EBA9ADCE404F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{580B3F30-1DBD-4438-AD19-EBA9ADCE404F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E65AB5EE-F2C8-4A8D-8D93-CCDA1E841F0F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BB4EF615-54DA-4A8A-8E99-B0FF27B7371C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="69">
   <si>
     <t>N</t>
   </si>
@@ -237,6 +237,12 @@
   </si>
   <si>
     <t>Code postal</t>
+  </si>
+  <si>
+    <t>Quantite_article</t>
+  </si>
+  <si>
+    <t>Quantite de chaque article dans la commande</t>
   </si>
 </sst>
 </file>
@@ -318,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -333,6 +339,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -390,8 +399,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D97F1EB4-EF69-4A77-9325-B5CC9874FEE7}" name="Tableau4234646" displayName="Tableau4234646" ref="A1:F36" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F36" xr:uid="{D97F1EB4-EF69-4A77-9325-B5CC9874FEE7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D97F1EB4-EF69-4A77-9325-B5CC9874FEE7}" name="Tableau4234646" displayName="Tableau4234646" ref="A1:F37" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F37" xr:uid="{D97F1EB4-EF69-4A77-9325-B5CC9874FEE7}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{A7585BCD-8D17-4F15-9C4B-7F44D4945DCF}" name="Name" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{9FC95855-C9FE-4C86-98B8-6295FE7C9BCA}" name="Type" dataDxfId="4"/>
@@ -701,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C508BB4-A982-4351-BEB9-D978C4430A2B}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I17:I18"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1298,6 +1307,22 @@
         <v>47</v>
       </c>
     </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>